<commit_message>
I am now able to copy columns from excel files. Need to add comments. Need to figure out keyerror 62
</commit_message>
<xml_diff>
--- a/Block data.xlsx
+++ b/Block data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E1231495\Desktop\coding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Documents\Code\excelOrganizer\excelOrganizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF2F3DE-D2EB-48E9-ADCA-399BEB35ED13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="10650"/>
+    <workbookView xWindow="29745" yWindow="1065" windowWidth="14400" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +36,6 @@
     <t>Cartridge part number</t>
   </si>
   <si>
-    <t>current carbon block part number</t>
-  </si>
-  <si>
     <t>current carbon block Description</t>
   </si>
   <si>
@@ -804,12 +802,15 @@
   </si>
   <si>
     <t>Follett FL4S</t>
+  </si>
+  <si>
+    <t>Current Carbon block part number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -896,7 +897,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4 3" xfId="1"/>
+    <cellStyle name="Normal 4 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1173,21 +1174,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1199,1204 +1200,1204 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="J3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="J4" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="J5" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
       <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
       <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
         <v>45</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
         <v>63</v>
       </c>
-      <c r="B13" t="s">
-        <v>64</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
         <v>71</v>
       </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
       <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
         <v>79</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
         <v>84</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
         <v>89</v>
       </c>
-      <c r="B19" t="s">
-        <v>90</v>
-      </c>
       <c r="C19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
         <v>91</v>
       </c>
-      <c r="B20" t="s">
-        <v>92</v>
-      </c>
       <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
         <v>93</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
         <v>98</v>
       </c>
-      <c r="B22" t="s">
-        <v>99</v>
-      </c>
       <c r="C22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
         <v>100</v>
       </c>
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
       <c r="C23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
         <v>102</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
         <v>107</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" t="s">
         <v>112</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" t="s">
         <v>117</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="D27" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="E27" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>121</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" t="s">
         <v>122</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>124</v>
-      </c>
       <c r="D28" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>121</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" t="s">
         <v>125</v>
       </c>
-      <c r="B29" t="s">
-        <v>126</v>
-      </c>
       <c r="C29" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D29" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>121</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" t="s">
         <v>127</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" t="s">
         <v>132</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" t="s">
         <v>137</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" t="s">
         <v>142</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" t="s">
         <v>147</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" t="s">
         <v>164</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" t="s">
         <v>169</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" t="s">
         <v>174</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" t="s">
         <v>179</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>183</v>
+      </c>
+      <c r="B43" t="s">
         <v>184</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" t="s">
         <v>189</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" t="s">
         <v>194</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B46" t="s">
         <v>199</v>
       </c>
-      <c r="B46" t="s">
-        <v>200</v>
-      </c>
       <c r="C46" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>200</v>
+      </c>
+      <c r="B47" t="s">
         <v>201</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>206</v>
+      </c>
+      <c r="B49" t="s">
         <v>207</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B50" t="s">
         <v>212</v>
       </c>
-      <c r="B50" t="s">
-        <v>213</v>
-      </c>
       <c r="C50" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="F50" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>213</v>
+      </c>
+      <c r="B51" t="s">
         <v>214</v>
       </c>
-      <c r="B51" t="s">
-        <v>215</v>
-      </c>
       <c r="C51" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>215</v>
+      </c>
+      <c r="B52" t="s">
         <v>216</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>220</v>
+      </c>
+      <c r="B53" t="s">
         <v>221</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="F53" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>225</v>
+      </c>
+      <c r="B54" t="s">
         <v>226</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>230</v>
+      </c>
+      <c r="B55" t="s">
         <v>231</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>235</v>
+      </c>
+      <c r="B56" t="s">
         <v>236</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="F56" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B57" t="s">
         <v>241</v>
       </c>
-      <c r="B57" t="s">
-        <v>242</v>
-      </c>
       <c r="C57" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="F57" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>242</v>
+      </c>
+      <c r="B58" t="s">
         <v>243</v>
       </c>
-      <c r="B58" t="s">
-        <v>244</v>
-      </c>
       <c r="C58" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="F58" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>244</v>
+      </c>
+      <c r="B59" t="s">
         <v>245</v>
       </c>
-      <c r="B59" t="s">
-        <v>246</v>
-      </c>
       <c r="C59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="F59" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" t="s">
         <v>247</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="F60" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>251</v>
+      </c>
+      <c r="B61" t="s">
         <v>252</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="F61" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="3"/>
@@ -2405,7 +2406,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -2416,7 +2417,7 @@
       <c r="F64" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:F63">
       <sortCondition ref="C1"/>
     </sortState>

</xml_diff>